<commit_message>
Update Route 101 encounters
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27920"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8AFD81-3E7F-4BF0-9D6A-6159BCDD1314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DAA5F2-07BC-4231-AA05-7757D8A41C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2550" yWindow="2550" windowWidth="15300" windowHeight="7875" activeTab="1" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="33">
   <si>
     <t>Location</t>
   </si>
@@ -64,6 +64,78 @@
   </si>
   <si>
     <t>Pokemon</t>
+  </si>
+  <si>
+    <t>Wurmple</t>
+  </si>
+  <si>
+    <t>Poochyena</t>
+  </si>
+  <si>
+    <t>Zigzagoon</t>
+  </si>
+  <si>
+    <t>Route 102</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Pikipek</t>
+  </si>
+  <si>
+    <t>Lotad</t>
+  </si>
+  <si>
+    <t>Ralts</t>
+  </si>
+  <si>
+    <t>Seedot</t>
+  </si>
+  <si>
+    <t>Marill</t>
+  </si>
+  <si>
+    <t>Goldeen</t>
+  </si>
+  <si>
+    <t>Magikarp</t>
+  </si>
+  <si>
+    <t>Corphish</t>
+  </si>
+  <si>
+    <t>Route 103</t>
+  </si>
+  <si>
+    <t>Wingull</t>
+  </si>
+  <si>
+    <t>Tentacool</t>
+  </si>
+  <si>
+    <t>Pelipper</t>
+  </si>
+  <si>
+    <t>Wailmer</t>
+  </si>
+  <si>
+    <t>Sharpedo</t>
+  </si>
+  <si>
+    <t>Route 104</t>
+  </si>
+  <si>
+    <t>Taillow</t>
+  </si>
+  <si>
+    <t>Route 105</t>
   </si>
 </sst>
 </file>
@@ -99,16 +171,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -124,6 +207,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
+<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
+  <bag type="Checkbox"/>
+  <bag type="XFControls">
+    <bagId k="CellControl">0</bagId>
+  </bag>
+  <bag type="XFComplement">
+    <bagId k="XFControls">1</bagId>
+  </bag>
+  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
+    <a k="MappedFeaturePropertyBags">
+      <bagId>2</bagId>
+    </a>
+  </bag>
+</FeaturePropertyBags>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -466,76 +566,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A925BAE-2E1E-4059-B9E1-CE8878C0DE7F}">
-  <dimension ref="A1:AH100"/>
+  <dimension ref="A1:AK100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="2" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2" t="s">
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2" t="s">
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1">
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4"/>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1">
         <v>0.2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="F2" s="1">
         <v>0.2</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.1</v>
       </c>
       <c r="G2" s="1">
         <v>0.1</v>
@@ -544,489 +648,885 @@
         <v>0.1</v>
       </c>
       <c r="I2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K2" s="1">
         <v>0.05</v>
       </c>
-      <c r="J2" s="1">
+      <c r="L2" s="1">
         <v>0.05</v>
       </c>
-      <c r="K2" s="1">
+      <c r="M2" s="1">
         <v>0.04</v>
       </c>
-      <c r="L2" s="1">
+      <c r="N2" s="1">
         <v>0.04</v>
       </c>
-      <c r="M2" s="1">
+      <c r="O2" s="1">
         <v>0.01</v>
       </c>
-      <c r="N2" s="1">
+      <c r="P2" s="1">
         <v>0.01</v>
       </c>
-      <c r="O2" s="1">
+      <c r="Q2" s="1">
         <v>0.6</v>
       </c>
-      <c r="P2" s="1">
+      <c r="R2" s="1">
         <v>0.3</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="S2" s="1">
         <v>0.05</v>
       </c>
-      <c r="R2" s="1">
+      <c r="T2" s="1">
         <v>0.04</v>
       </c>
-      <c r="S2" s="1">
+      <c r="U2" s="1">
         <v>0.01</v>
       </c>
-      <c r="T2" s="1">
+      <c r="V2" s="1">
         <v>0.6</v>
       </c>
-      <c r="U2" s="1">
+      <c r="W2" s="1">
         <v>0.3</v>
       </c>
-      <c r="V2" s="1">
+      <c r="X2" s="1">
         <v>0.05</v>
       </c>
-      <c r="W2" s="1">
+      <c r="Y2" s="1">
         <v>0.04</v>
       </c>
-      <c r="X2" s="1">
+      <c r="Z2" s="1">
         <v>0.01</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="AA2" s="1">
         <v>0.7</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="AB2" s="1">
         <v>0.3</v>
       </c>
-      <c r="AA2" s="1">
+      <c r="AC2" s="1">
         <v>0.6</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AD2" s="1">
         <v>0.2</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AE2" s="1">
         <v>0.2</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AF2" s="1">
         <v>0.4</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AG2" s="1">
         <v>0.4</v>
       </c>
-      <c r="AF2" s="1">
+      <c r="AH2" s="1">
         <v>0.15</v>
       </c>
-      <c r="AG2" s="1">
+      <c r="AI2" s="1">
         <v>0.04</v>
       </c>
-      <c r="AH2" s="1">
+      <c r="AJ2" s="1">
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+      <c r="B3" s="3"/>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK3" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" t="s">
+        <v>20</v>
+      </c>
+      <c r="T4" t="s">
+        <v>20</v>
+      </c>
+      <c r="U4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" t="s">
+        <v>25</v>
+      </c>
+      <c r="S5" t="s">
+        <v>25</v>
+      </c>
+      <c r="T5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>25</v>
+      </c>
+      <c r="R6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S6" t="s">
+        <v>25</v>
+      </c>
+      <c r="T6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4"/>
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4"/>
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4"/>
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" s="4"/>
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
-      <c r="B83" s="4"/>
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
-      <c r="B84" s="4"/>
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4"/>
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
-      <c r="B86" s="4"/>
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4"/>
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4"/>
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4"/>
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
-      <c r="B93" s="4"/>
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4"/>
+      <c r="A94" s="3"/>
+      <c r="B94" s="3"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
-      <c r="B95" s="4"/>
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
-      <c r="B96" s="4"/>
+      <c r="A96" s="3"/>
+      <c r="B96" s="3"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
+      <c r="A97" s="3"/>
+      <c r="B97" s="3"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
-      <c r="B98" s="4"/>
+      <c r="A98" s="3"/>
+      <c r="B98" s="3"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
+      <c r="A100" s="3"/>
+      <c r="B100" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="105">
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
+  <mergeCells count="106">
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
     <mergeCell ref="A86:B86"/>
     <mergeCell ref="A87:B87"/>
     <mergeCell ref="A88:B88"/>
@@ -1039,90 +1539,15 @@
     <mergeCell ref="A83:B83"/>
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="AD1:AH1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:N1"/>
-    <mergeCell ref="O1:S1"/>
-    <mergeCell ref="T1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AC1"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fill in regional dex in docs
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DAA5F2-07BC-4231-AA05-7757D8A41C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0640C164-2F45-4974-8610-DB4296CAAB36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2550" windowWidth="15300" windowHeight="7875" activeTab="1" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
+    <workbookView xWindow="2550" yWindow="2550" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
   <sheets>
     <sheet name="Regional Dex" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="276">
   <si>
     <t>Location</t>
   </si>
@@ -136,6 +136,735 @@
   </si>
   <si>
     <t>Route 105</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Treecko</t>
+  </si>
+  <si>
+    <t>Grovyle</t>
+  </si>
+  <si>
+    <t>Sceptile</t>
+  </si>
+  <si>
+    <t>Torchic</t>
+  </si>
+  <si>
+    <t>Combusken</t>
+  </si>
+  <si>
+    <t>Blaziken</t>
+  </si>
+  <si>
+    <t>Mudkip</t>
+  </si>
+  <si>
+    <t>Marshtomp</t>
+  </si>
+  <si>
+    <t>Swampert</t>
+  </si>
+  <si>
+    <t>Mightyena</t>
+  </si>
+  <si>
+    <t>Linoone</t>
+  </si>
+  <si>
+    <t>Obstagoon</t>
+  </si>
+  <si>
+    <t>Silcoon</t>
+  </si>
+  <si>
+    <t>Beautifly</t>
+  </si>
+  <si>
+    <t>Cascoon</t>
+  </si>
+  <si>
+    <t>Dustox</t>
+  </si>
+  <si>
+    <t>Lombre</t>
+  </si>
+  <si>
+    <t>Ludicolo</t>
+  </si>
+  <si>
+    <t>Nuzleaf</t>
+  </si>
+  <si>
+    <t>Shiftry</t>
+  </si>
+  <si>
+    <t>Poliwag</t>
+  </si>
+  <si>
+    <t>Poliwhirl</t>
+  </si>
+  <si>
+    <t>Poliwrath</t>
+  </si>
+  <si>
+    <t>Politoed</t>
+  </si>
+  <si>
+    <t>Swellow</t>
+  </si>
+  <si>
+    <t>Kirlia</t>
+  </si>
+  <si>
+    <t>Gardevoir</t>
+  </si>
+  <si>
+    <t>Gallade</t>
+  </si>
+  <si>
+    <t>Trumbeak</t>
+  </si>
+  <si>
+    <t>Toucannon</t>
+  </si>
+  <si>
+    <t>Surskit</t>
+  </si>
+  <si>
+    <t>Masquerain</t>
+  </si>
+  <si>
+    <t>Foongus</t>
+  </si>
+  <si>
+    <t>Amoonguss</t>
+  </si>
+  <si>
+    <t>Shroomish</t>
+  </si>
+  <si>
+    <t>Breloom</t>
+  </si>
+  <si>
+    <t>Slakoth</t>
+  </si>
+  <si>
+    <t>Vigoroth</t>
+  </si>
+  <si>
+    <t>Slaking</t>
+  </si>
+  <si>
+    <t>Mankey</t>
+  </si>
+  <si>
+    <t>Primeape</t>
+  </si>
+  <si>
+    <t>Annihilape</t>
+  </si>
+  <si>
+    <t>Nincada</t>
+  </si>
+  <si>
+    <t>Ninjask</t>
+  </si>
+  <si>
+    <t>Shedinja</t>
+  </si>
+  <si>
+    <t>Whismur</t>
+  </si>
+  <si>
+    <t>Loudred</t>
+  </si>
+  <si>
+    <t>Exploud</t>
+  </si>
+  <si>
+    <t>Makuhita</t>
+  </si>
+  <si>
+    <t>Hariyama</t>
+  </si>
+  <si>
+    <t>Seaking</t>
+  </si>
+  <si>
+    <t>Gyarados</t>
+  </si>
+  <si>
+    <t>Shellos</t>
+  </si>
+  <si>
+    <t>Gastrodon</t>
+  </si>
+  <si>
+    <t>Azurill</t>
+  </si>
+  <si>
+    <t>Azumarill</t>
+  </si>
+  <si>
+    <t>Geodude</t>
+  </si>
+  <si>
+    <t>Graveler</t>
+  </si>
+  <si>
+    <t>Golem</t>
+  </si>
+  <si>
+    <t>Roggenrola</t>
+  </si>
+  <si>
+    <t>Boldore</t>
+  </si>
+  <si>
+    <t>Gigalith</t>
+  </si>
+  <si>
+    <t>Silicobra</t>
+  </si>
+  <si>
+    <t>Sandaconda</t>
+  </si>
+  <si>
+    <t>Nosepass</t>
+  </si>
+  <si>
+    <t>Probopass</t>
+  </si>
+  <si>
+    <t>Skitty</t>
+  </si>
+  <si>
+    <t>Delcatty</t>
+  </si>
+  <si>
+    <t>Zubat</t>
+  </si>
+  <si>
+    <t>Golbat</t>
+  </si>
+  <si>
+    <t>Crobat</t>
+  </si>
+  <si>
+    <t>Oricorio</t>
+  </si>
+  <si>
+    <t>Tentacruel</t>
+  </si>
+  <si>
+    <t>Frillish</t>
+  </si>
+  <si>
+    <t>Jellicent</t>
+  </si>
+  <si>
+    <t>Mareanie</t>
+  </si>
+  <si>
+    <t>Toxapex</t>
+  </si>
+  <si>
+    <t>Misdreavus</t>
+  </si>
+  <si>
+    <t>Mismagius</t>
+  </si>
+  <si>
+    <t>Sableye</t>
+  </si>
+  <si>
+    <t>Mawile</t>
+  </si>
+  <si>
+    <t>Carbink</t>
+  </si>
+  <si>
+    <t>Rockruff</t>
+  </si>
+  <si>
+    <t>Lycanroc</t>
+  </si>
+  <si>
+    <t>Aron</t>
+  </si>
+  <si>
+    <t>Lairon</t>
+  </si>
+  <si>
+    <t>Aggron</t>
+  </si>
+  <si>
+    <t>Meditite</t>
+  </si>
+  <si>
+    <t>Medicham</t>
+  </si>
+  <si>
+    <t>Electrike</t>
+  </si>
+  <si>
+    <t>Manectric</t>
+  </si>
+  <si>
+    <t>Plusle</t>
+  </si>
+  <si>
+    <t>Minun</t>
+  </si>
+  <si>
+    <t>Magnemite</t>
+  </si>
+  <si>
+    <t>Magneton</t>
+  </si>
+  <si>
+    <t>Magnezone</t>
+  </si>
+  <si>
+    <t>Volbeat</t>
+  </si>
+  <si>
+    <t>Illumise</t>
+  </si>
+  <si>
+    <t>Oddish</t>
+  </si>
+  <si>
+    <t>Gloom</t>
+  </si>
+  <si>
+    <t>Vileplume</t>
+  </si>
+  <si>
+    <t>Bellossom</t>
+  </si>
+  <si>
+    <t>Doduo</t>
+  </si>
+  <si>
+    <t>Dodrio</t>
+  </si>
+  <si>
+    <t>Budew</t>
+  </si>
+  <si>
+    <t>Roselia</t>
+  </si>
+  <si>
+    <t>Roserade</t>
+  </si>
+  <si>
+    <t>Gulpin</t>
+  </si>
+  <si>
+    <t>Swalot</t>
+  </si>
+  <si>
+    <t>Carvanha</t>
+  </si>
+  <si>
+    <t>Wailord</t>
+  </si>
+  <si>
+    <t>Numel</t>
+  </si>
+  <si>
+    <t>Camerupt</t>
+  </si>
+  <si>
+    <t>Darumaka</t>
+  </si>
+  <si>
+    <t>Darmanitan</t>
+  </si>
+  <si>
+    <t>Slugma</t>
+  </si>
+  <si>
+    <t>Magcargo</t>
+  </si>
+  <si>
+    <t>Torkoal</t>
+  </si>
+  <si>
+    <t>Salandit</t>
+  </si>
+  <si>
+    <t>Salazzle</t>
+  </si>
+  <si>
+    <t>Spoink</t>
+  </si>
+  <si>
+    <t>Grumpig</t>
+  </si>
+  <si>
+    <t>Sandshrew</t>
+  </si>
+  <si>
+    <t>Sandslash</t>
+  </si>
+  <si>
+    <t>Sandygast</t>
+  </si>
+  <si>
+    <t>Palossand</t>
+  </si>
+  <si>
+    <t>Spinda</t>
+  </si>
+  <si>
+    <t>Skarmory</t>
+  </si>
+  <si>
+    <t>Helioptile</t>
+  </si>
+  <si>
+    <t>Heliolisk</t>
+  </si>
+  <si>
+    <t>Trapinch</t>
+  </si>
+  <si>
+    <t>Vibrava</t>
+  </si>
+  <si>
+    <t>Flygon</t>
+  </si>
+  <si>
+    <t>Hippopotas</t>
+  </si>
+  <si>
+    <t>Hippowdon</t>
+  </si>
+  <si>
+    <t>Cacnea</t>
+  </si>
+  <si>
+    <t>Cacturne</t>
+  </si>
+  <si>
+    <t>Exeggcute</t>
+  </si>
+  <si>
+    <t>Exeggutor</t>
+  </si>
+  <si>
+    <t>Swablu</t>
+  </si>
+  <si>
+    <t>Altaria</t>
+  </si>
+  <si>
+    <t>Zangoose</t>
+  </si>
+  <si>
+    <t>Seviper</t>
+  </si>
+  <si>
+    <t>Lunatone</t>
+  </si>
+  <si>
+    <t>Solrock</t>
+  </si>
+  <si>
+    <t>Barboach</t>
+  </si>
+  <si>
+    <t>Whiscash</t>
+  </si>
+  <si>
+    <t>Crawdaunt</t>
+  </si>
+  <si>
+    <t>Mantyke</t>
+  </si>
+  <si>
+    <t>Mantine</t>
+  </si>
+  <si>
+    <t>Baltoy</t>
+  </si>
+  <si>
+    <t>Claydol</t>
+  </si>
+  <si>
+    <t>Lileep</t>
+  </si>
+  <si>
+    <t>Cradily</t>
+  </si>
+  <si>
+    <t>Anorith</t>
+  </si>
+  <si>
+    <t>Armaldo</t>
+  </si>
+  <si>
+    <t>Minior</t>
+  </si>
+  <si>
+    <t>Feebas</t>
+  </si>
+  <si>
+    <t>Milotic</t>
+  </si>
+  <si>
+    <t>Castform</t>
+  </si>
+  <si>
+    <t>Staryu</t>
+  </si>
+  <si>
+    <t>Starmie</t>
+  </si>
+  <si>
+    <t>Kecleon</t>
+  </si>
+  <si>
+    <t>Shuppet</t>
+  </si>
+  <si>
+    <t>Banette</t>
+  </si>
+  <si>
+    <t>Duskull</t>
+  </si>
+  <si>
+    <t>Dusclops</t>
+  </si>
+  <si>
+    <t>Dusknoir</t>
+  </si>
+  <si>
+    <t>Tropius</t>
+  </si>
+  <si>
+    <t>Chingling</t>
+  </si>
+  <si>
+    <t>Chimecho</t>
+  </si>
+  <si>
+    <t>Absol</t>
+  </si>
+  <si>
+    <t>Vulpix</t>
+  </si>
+  <si>
+    <t>Ninetales</t>
+  </si>
+  <si>
+    <t>Pichu</t>
+  </si>
+  <si>
+    <t>Pikachu</t>
+  </si>
+  <si>
+    <t>Raichu</t>
+  </si>
+  <si>
+    <t>Wynaut</t>
+  </si>
+  <si>
+    <t>Wobbuffet</t>
+  </si>
+  <si>
+    <t>Natu</t>
+  </si>
+  <si>
+    <t>Xatu</t>
+  </si>
+  <si>
+    <t>Girafarig</t>
+  </si>
+  <si>
+    <t>Farigiraf</t>
+  </si>
+  <si>
+    <t>Phanpy</t>
+  </si>
+  <si>
+    <t>Donphan</t>
+  </si>
+  <si>
+    <t>Pinsir</t>
+  </si>
+  <si>
+    <t>Heracross</t>
+  </si>
+  <si>
+    <t>Scyther</t>
+  </si>
+  <si>
+    <t>Scizor</t>
+  </si>
+  <si>
+    <t>Kleavor</t>
+  </si>
+  <si>
+    <t>Yanma</t>
+  </si>
+  <si>
+    <t>Yanmega</t>
+  </si>
+  <si>
+    <t>Rhyhorn</t>
+  </si>
+  <si>
+    <t>Rhydon</t>
+  </si>
+  <si>
+    <t>Rhyperior</t>
+  </si>
+  <si>
+    <t>Sneasel</t>
+  </si>
+  <si>
+    <t>Weavile</t>
+  </si>
+  <si>
+    <t>Snorunt</t>
+  </si>
+  <si>
+    <t>Glalie</t>
+  </si>
+  <si>
+    <t>Froslass</t>
+  </si>
+  <si>
+    <t>Spheal</t>
+  </si>
+  <si>
+    <t>Sealeo</t>
+  </si>
+  <si>
+    <t>Walrein</t>
+  </si>
+  <si>
+    <t>Crabrawler</t>
+  </si>
+  <si>
+    <t>Crabominable</t>
+  </si>
+  <si>
+    <t>Clamperl</t>
+  </si>
+  <si>
+    <t>Huntail</t>
+  </si>
+  <si>
+    <t>Gorebyss</t>
+  </si>
+  <si>
+    <t>Relicanth</t>
+  </si>
+  <si>
+    <t>Corsola</t>
+  </si>
+  <si>
+    <t>Cursola</t>
+  </si>
+  <si>
+    <t>Chinchou</t>
+  </si>
+  <si>
+    <t>Lanturn</t>
+  </si>
+  <si>
+    <t>Tynamo</t>
+  </si>
+  <si>
+    <t>Eelektrik</t>
+  </si>
+  <si>
+    <t>Eelektross</t>
+  </si>
+  <si>
+    <t>Remoraid</t>
+  </si>
+  <si>
+    <t>Octillery</t>
+  </si>
+  <si>
+    <t>Luvdisc</t>
+  </si>
+  <si>
+    <t>Alomomola</t>
+  </si>
+  <si>
+    <t>Horsea</t>
+  </si>
+  <si>
+    <t>Seadra</t>
+  </si>
+  <si>
+    <t>Kingdra</t>
+  </si>
+  <si>
+    <t>Bagon</t>
+  </si>
+  <si>
+    <t>Shelgon</t>
+  </si>
+  <si>
+    <t>Salamence</t>
+  </si>
+  <si>
+    <t>Beldum</t>
+  </si>
+  <si>
+    <t>Metang</t>
+  </si>
+  <si>
+    <t>Metagross</t>
+  </si>
+  <si>
+    <t>Larvitar</t>
+  </si>
+  <si>
+    <t>Pupitar</t>
+  </si>
+  <si>
+    <t>Tyranitar</t>
+  </si>
+  <si>
+    <t>Regirock</t>
+  </si>
+  <si>
+    <t>Regice</t>
+  </si>
+  <si>
+    <t>Registeel</t>
+  </si>
+  <si>
+    <t>Latias</t>
+  </si>
+  <si>
+    <t>Latios</t>
+  </si>
+  <si>
+    <t>Kyogre</t>
+  </si>
+  <si>
+    <t>Groudon</t>
+  </si>
+  <si>
+    <t>Rayquaza</t>
+  </si>
+  <si>
+    <t>Jirachi</t>
+  </si>
+  <si>
+    <t>Deoxys</t>
   </si>
 </sst>
 </file>
@@ -171,26 +900,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
           <xfpb:xfComplement i="0"/>
         </ext>
       </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,20 +1271,2103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C261"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>179</v>
+      </c>
+      <c r="B180" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>180</v>
+      </c>
+      <c r="B181" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>181</v>
+      </c>
+      <c r="B182" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>186</v>
+      </c>
+      <c r="B187" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>187</v>
+      </c>
+      <c r="B188" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>188</v>
+      </c>
+      <c r="B189" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>189</v>
+      </c>
+      <c r="B190" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>190</v>
+      </c>
+      <c r="B191" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>191</v>
+      </c>
+      <c r="B192" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>192</v>
+      </c>
+      <c r="B193" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>193</v>
+      </c>
+      <c r="B194" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>194</v>
+      </c>
+      <c r="B195" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>195</v>
+      </c>
+      <c r="B196" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>196</v>
+      </c>
+      <c r="B197" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>197</v>
+      </c>
+      <c r="B198" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>198</v>
+      </c>
+      <c r="B199" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>199</v>
+      </c>
+      <c r="B200" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>200</v>
+      </c>
+      <c r="B201" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>203</v>
+      </c>
+      <c r="B204" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>204</v>
+      </c>
+      <c r="B205" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>209</v>
+      </c>
+      <c r="B210" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>210</v>
+      </c>
+      <c r="B211" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>211</v>
+      </c>
+      <c r="B212" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>212</v>
+      </c>
+      <c r="B213" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>213</v>
+      </c>
+      <c r="B214" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>214</v>
+      </c>
+      <c r="B215" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>215</v>
+      </c>
+      <c r="B216" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>216</v>
+      </c>
+      <c r="B217" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>217</v>
+      </c>
+      <c r="B218" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>218</v>
+      </c>
+      <c r="B219" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>219</v>
+      </c>
+      <c r="B220" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>220</v>
+      </c>
+      <c r="B221" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>221</v>
+      </c>
+      <c r="B222" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>222</v>
+      </c>
+      <c r="B223" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>223</v>
+      </c>
+      <c r="B224" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>224</v>
+      </c>
+      <c r="B225" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>225</v>
+      </c>
+      <c r="B226" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>226</v>
+      </c>
+      <c r="B227" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>227</v>
+      </c>
+      <c r="B228" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>228</v>
+      </c>
+      <c r="B229" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>229</v>
+      </c>
+      <c r="B230" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>230</v>
+      </c>
+      <c r="B231" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>231</v>
+      </c>
+      <c r="B232" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>232</v>
+      </c>
+      <c r="B233" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>233</v>
+      </c>
+      <c r="B234" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>234</v>
+      </c>
+      <c r="B235" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>235</v>
+      </c>
+      <c r="B236" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>236</v>
+      </c>
+      <c r="B237" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>237</v>
+      </c>
+      <c r="B238" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>238</v>
+      </c>
+      <c r="B239" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>239</v>
+      </c>
+      <c r="B240" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>240</v>
+      </c>
+      <c r="B241" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>241</v>
+      </c>
+      <c r="B242" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>242</v>
+      </c>
+      <c r="B243" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>243</v>
+      </c>
+      <c r="B244" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>244</v>
+      </c>
+      <c r="B245" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>245</v>
+      </c>
+      <c r="B246" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>246</v>
+      </c>
+      <c r="B247" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>247</v>
+      </c>
+      <c r="B248" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>248</v>
+      </c>
+      <c r="B249" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>249</v>
+      </c>
+      <c r="B250" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>250</v>
+      </c>
+      <c r="B251" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>251</v>
+      </c>
+      <c r="B252" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>252</v>
+      </c>
+      <c r="B253" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>253</v>
+      </c>
+      <c r="B254" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>254</v>
+      </c>
+      <c r="B255" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>255</v>
+      </c>
+      <c r="B256" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>256</v>
+      </c>
+      <c r="B257" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>257</v>
+      </c>
+      <c r="B258" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>258</v>
+      </c>
+      <c r="B259" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>259</v>
+      </c>
+      <c r="B260" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>260</v>
+      </c>
+      <c r="B261" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -568,8 +3379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A925BAE-2E1E-4059-B9E1-CE8878C0DE7F}">
   <dimension ref="A1:AK100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,20 +3392,20 @@
         <v>15</v>
       </c>
       <c r="D1" s="4"/>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
       <c r="Q1" s="4" t="s">
         <v>2</v>
       </c>
@@ -733,10 +3544,10 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="5"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -779,15 +3590,15 @@
       <c r="P3" t="s">
         <v>16</v>
       </c>
-      <c r="AK3" s="7" t="b">
+      <c r="AK3" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="5"/>
       <c r="C4">
         <v>3</v>
       </c>
@@ -877,10 +3688,10 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="5"/>
       <c r="C5">
         <v>2</v>
       </c>
@@ -970,10 +3781,10 @@
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="5"/>
       <c r="C6">
         <v>3</v>
       </c>
@@ -1063,385 +3874,478 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="5"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
+      <c r="A78" s="5"/>
+      <c r="B78" s="5"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="3"/>
-      <c r="B83" s="3"/>
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3"/>
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="3"/>
-      <c r="B89" s="3"/>
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="3"/>
-      <c r="B90" s="3"/>
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="3"/>
-      <c r="B91" s="3"/>
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="3"/>
-      <c r="B92" s="3"/>
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="3"/>
-      <c r="B93" s="3"/>
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="3"/>
-      <c r="B94" s="3"/>
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="3"/>
-      <c r="B95" s="3"/>
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="3"/>
-      <c r="B96" s="3"/>
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="3"/>
-      <c r="B97" s="3"/>
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="3"/>
-      <c r="B98" s="3"/>
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="3"/>
-      <c r="B99" s="3"/>
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="3"/>
-      <c r="B100" s="3"/>
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="106">
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
@@ -1455,99 +4359,6 @@
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update docs to track completed species
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27920"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2168A937-6D76-4C7C-BA2D-614E3359DC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C53FAD-7ADB-4579-86BC-4E685840D3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2550" yWindow="2550" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="280">
-  <si>
-    <t>Location</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="282">
   <si>
     <t>Land</t>
   </si>
@@ -877,6 +874,15 @@
   </si>
   <si>
     <t>Dragon</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Abilities</t>
   </si>
 </sst>
 </file>
@@ -925,10 +931,10 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1283,289 +1289,355 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
-  <dimension ref="A1:E260"/>
+  <dimension ref="A1:F260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
+      <selection activeCell="C260" sqref="C260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>279</v>
       </c>
       <c r="D1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E1" t="s">
         <v>276</v>
       </c>
-      <c r="E1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>280</v>
       </c>
       <c r="D3" t="s">
+        <v>277</v>
+      </c>
+      <c r="E3" t="s">
         <v>278</v>
       </c>
-      <c r="E3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>280</v>
       </c>
       <c r="D4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E4" t="s">
         <v>278</v>
       </c>
-      <c r="E4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1573,7 +1645,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1581,7 +1653,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1589,7 +1661,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1597,7 +1669,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1605,7 +1677,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1613,7 +1685,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1621,7 +1693,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1629,7 +1701,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1637,7 +1709,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1645,7 +1717,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1653,7 +1725,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1661,7 +1733,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1669,7 +1741,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1677,7 +1749,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1685,7 +1757,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1693,7 +1765,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1701,7 +1773,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1709,7 +1781,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1717,7 +1789,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1725,7 +1797,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1733,7 +1805,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1741,7 +1813,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1749,7 +1821,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1757,7 +1829,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1765,7 +1837,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1773,7 +1845,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1781,7 +1853,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1789,7 +1861,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1797,7 +1869,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1805,7 +1877,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1813,7 +1885,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1821,7 +1893,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1829,7 +1901,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1837,7 +1909,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1845,7 +1917,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1853,7 +1925,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1861,7 +1933,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1869,7 +1941,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1877,7 +1949,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1885,7 +1957,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1893,7 +1965,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1901,7 +1973,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1909,7 +1981,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1917,7 +1989,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1925,7 +1997,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1933,7 +2005,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1941,7 +2013,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1949,7 +2021,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1957,7 +2029,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1965,7 +2037,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1973,7 +2045,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1981,7 +2053,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1989,7 +2061,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1997,7 +2069,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -2005,7 +2077,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2013,7 +2085,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -2021,7 +2093,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2029,7 +2101,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2037,7 +2109,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2045,7 +2117,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2053,7 +2125,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2061,7 +2133,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2069,7 +2141,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -2077,7 +2149,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2085,7 +2157,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -2093,7 +2165,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -2101,7 +2173,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2109,7 +2181,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2117,7 +2189,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -2125,7 +2197,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2133,7 +2205,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2141,7 +2213,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2149,7 +2221,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2157,7 +2229,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2165,7 +2237,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2173,7 +2245,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2181,7 +2253,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -2189,7 +2261,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -2197,7 +2269,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2205,7 +2277,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -2213,7 +2285,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -2221,7 +2293,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2229,7 +2301,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -2237,7 +2309,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -2245,7 +2317,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -2253,7 +2325,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -2261,7 +2333,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -2269,7 +2341,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -2277,7 +2349,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -2285,7 +2357,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -2293,7 +2365,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2301,7 +2373,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -2309,7 +2381,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -2317,7 +2389,7 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2325,7 +2397,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -2333,7 +2405,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -2341,7 +2413,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2349,7 +2421,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -2357,7 +2429,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -2365,7 +2437,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -2373,7 +2445,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -2381,7 +2453,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -2389,7 +2461,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -2397,7 +2469,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -2405,7 +2477,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -2413,7 +2485,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -2421,7 +2493,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -2429,7 +2501,7 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -2437,7 +2509,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -2445,7 +2517,7 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -2453,7 +2525,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -2461,7 +2533,7 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -2469,7 +2541,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -2477,7 +2549,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -2485,7 +2557,7 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -2493,7 +2565,7 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -2501,7 +2573,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -2509,7 +2581,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -2517,7 +2589,7 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -2525,7 +2597,7 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -2533,7 +2605,7 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -2541,7 +2613,7 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -2549,7 +2621,7 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -2557,7 +2629,7 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -2565,7 +2637,7 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -2573,7 +2645,7 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -2581,7 +2653,7 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -2589,7 +2661,7 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -2597,7 +2669,7 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -2605,7 +2677,7 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -2613,7 +2685,7 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -2621,7 +2693,7 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -2629,7 +2701,7 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -2637,7 +2709,7 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -2645,7 +2717,7 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -2653,7 +2725,7 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -2661,7 +2733,7 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -2669,7 +2741,7 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -2677,7 +2749,7 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -2685,7 +2757,7 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -2693,7 +2765,7 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -2701,7 +2773,7 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -2709,7 +2781,7 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -2717,7 +2789,7 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -2725,7 +2797,7 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -2733,7 +2805,7 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -2741,7 +2813,7 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -2749,7 +2821,7 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -2757,7 +2829,7 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -2765,7 +2837,7 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -2773,7 +2845,7 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -2781,7 +2853,7 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -2789,7 +2861,7 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -2797,7 +2869,7 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -2805,7 +2877,7 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -2813,7 +2885,7 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -2821,7 +2893,7 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -2829,7 +2901,7 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -2837,7 +2909,7 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -2845,7 +2917,7 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -2853,7 +2925,7 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -2861,7 +2933,7 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -2869,7 +2941,7 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -2877,7 +2949,7 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -2885,7 +2957,7 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -2893,7 +2965,7 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -2901,7 +2973,7 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -2909,7 +2981,7 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -2917,7 +2989,7 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -2925,7 +2997,7 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -2933,7 +3005,7 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -2941,7 +3013,7 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -2949,7 +3021,7 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
@@ -2957,7 +3029,7 @@
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
@@ -2965,7 +3037,7 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -2973,7 +3045,7 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
@@ -2981,7 +3053,7 @@
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
@@ -2989,7 +3061,7 @@
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
@@ -2997,7 +3069,7 @@
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -3005,7 +3077,7 @@
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
@@ -3013,7 +3085,7 @@
         <v>212</v>
       </c>
       <c r="B213" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
@@ -3021,7 +3093,7 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
@@ -3029,7 +3101,7 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
@@ -3037,7 +3109,7 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
@@ -3045,7 +3117,7 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
@@ -3053,7 +3125,7 @@
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
@@ -3061,7 +3133,7 @@
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -3069,7 +3141,7 @@
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
@@ -3077,7 +3149,7 @@
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
@@ -3085,7 +3157,7 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
@@ -3093,7 +3165,7 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
@@ -3101,7 +3173,7 @@
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
@@ -3109,7 +3181,7 @@
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
@@ -3117,7 +3189,7 @@
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
@@ -3125,7 +3197,7 @@
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
@@ -3133,7 +3205,7 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
@@ -3141,7 +3213,7 @@
         <v>228</v>
       </c>
       <c r="B229" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
@@ -3149,7 +3221,7 @@
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
@@ -3157,7 +3229,7 @@
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -3165,7 +3237,7 @@
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
@@ -3173,7 +3245,7 @@
         <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
@@ -3181,7 +3253,7 @@
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -3189,7 +3261,7 @@
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
@@ -3197,7 +3269,7 @@
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
@@ -3205,7 +3277,7 @@
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -3213,7 +3285,7 @@
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
@@ -3221,7 +3293,7 @@
         <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
@@ -3229,7 +3301,7 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
@@ -3237,7 +3309,7 @@
         <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
@@ -3245,7 +3317,7 @@
         <v>241</v>
       </c>
       <c r="B242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
@@ -3253,7 +3325,7 @@
         <v>242</v>
       </c>
       <c r="B243" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
@@ -3261,7 +3333,7 @@
         <v>243</v>
       </c>
       <c r="B244" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
@@ -3269,7 +3341,7 @@
         <v>244</v>
       </c>
       <c r="B245" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
@@ -3277,7 +3349,7 @@
         <v>245</v>
       </c>
       <c r="B246" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -3285,7 +3357,7 @@
         <v>246</v>
       </c>
       <c r="B247" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
@@ -3293,7 +3365,7 @@
         <v>247</v>
       </c>
       <c r="B248" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
@@ -3301,7 +3373,7 @@
         <v>248</v>
       </c>
       <c r="B249" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
@@ -3309,7 +3381,7 @@
         <v>249</v>
       </c>
       <c r="B250" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
@@ -3317,7 +3389,7 @@
         <v>250</v>
       </c>
       <c r="B251" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
@@ -3325,7 +3397,7 @@
         <v>251</v>
       </c>
       <c r="B252" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
@@ -3333,7 +3405,7 @@
         <v>252</v>
       </c>
       <c r="B253" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
@@ -3341,7 +3413,7 @@
         <v>253</v>
       </c>
       <c r="B254" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
@@ -3349,7 +3421,7 @@
         <v>254</v>
       </c>
       <c r="B255" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
@@ -3357,7 +3429,7 @@
         <v>255</v>
       </c>
       <c r="B256" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
@@ -3365,7 +3437,7 @@
         <v>256</v>
       </c>
       <c r="B257" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
@@ -3373,7 +3445,7 @@
         <v>257</v>
       </c>
       <c r="B258" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
@@ -3381,7 +3453,7 @@
         <v>258</v>
       </c>
       <c r="B259" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
@@ -3389,7 +3461,7 @@
         <v>259</v>
       </c>
       <c r="B260" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -3408,14 +3480,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="4"/>
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="5"/>
       <c r="E1" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -3428,45 +3500,45 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="E2" s="1">
         <v>0.2</v>
@@ -3566,10 +3638,10 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="5"/>
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -3577,50 +3649,50 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>10</v>
       </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AK3" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="5"/>
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="4"/>
       <c r="C4">
         <v>2</v>
       </c>
@@ -3628,92 +3700,92 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
+      <c r="K4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="s">
+      <c r="L4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" t="s">
         <v>25</v>
       </c>
-      <c r="J4" t="s">
+      <c r="R4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" t="s">
-        <v>25</v>
-      </c>
-      <c r="T4" t="s">
-        <v>27</v>
-      </c>
-      <c r="U4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5">
         <v>3</v>
       </c>
@@ -3721,92 +3793,92 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="L5" t="s">
         <v>10</v>
       </c>
-      <c r="H5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="M5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P5" t="s">
         <v>18</v>
       </c>
-      <c r="O5" t="s">
-        <v>11</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5" t="s">
+        <v>19</v>
+      </c>
+      <c r="T5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" t="s">
         <v>20</v>
       </c>
-      <c r="R5" t="s">
+      <c r="AA5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB5" t="s">
         <v>20</v>
       </c>
-      <c r="S5" t="s">
+      <c r="AC5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD5" t="s">
         <v>20</v>
       </c>
-      <c r="T5" t="s">
-        <v>20</v>
-      </c>
-      <c r="U5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA5" t="s">
+      <c r="AE5" t="s">
         <v>22</v>
       </c>
-      <c r="AB5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC5" t="s">
+      <c r="AF5" t="s">
         <v>22</v>
       </c>
-      <c r="AD5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>23</v>
-      </c>
       <c r="AG5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AH5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AI5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AJ5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="5"/>
+      <c r="A6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="4"/>
       <c r="C6">
         <v>3</v>
       </c>
@@ -3814,557 +3886,467 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="T6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AB6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AC6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AD6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AE6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AF6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AG6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AH6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AI6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AJ6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="B7" s="5"/>
+      <c r="A7" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="5"/>
-      <c r="B77" s="5"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="5"/>
-      <c r="B78" s="5"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
-      <c r="B85" s="5"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
-      <c r="B86" s="5"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-      <c r="B87" s="5"/>
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="B89" s="5"/>
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="5"/>
-      <c r="B95" s="5"/>
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="5"/>
-      <c r="B96" s="5"/>
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="5"/>
-      <c r="B97" s="5"/>
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-      <c r="B98" s="5"/>
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="5"/>
-      <c r="B99" s="5"/>
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="5"/>
-      <c r="B100" s="5"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="106">
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
     <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
@@ -4381,6 +4363,96 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Route 102 and Route 103 wild encounters
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C53FAD-7ADB-4579-86BC-4E685840D3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CF7CD2-F542-47F4-9A3F-B77A72F0D040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2550" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
+    <workbookView xWindow="2550" yWindow="2550" windowWidth="15300" windowHeight="7875" activeTab="1" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
   <sheets>
     <sheet name="Regional Dex" sheetId="2" r:id="rId1"/>
@@ -931,10 +931,10 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1291,9 +1291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
   <dimension ref="A1:F260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
-      <selection activeCell="C260" sqref="C260"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3473,19 +3471,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A925BAE-2E1E-4059-B9E1-CE8878C0DE7F}">
   <dimension ref="A1:AK100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="4"/>
       <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3500,40 +3498,40 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5" t="s">
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5" t="s">
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5" t="s">
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5" t="s">
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3638,10 +3636,10 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="5"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -3689,12 +3687,12 @@
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="5"/>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -3706,10 +3704,10 @@
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>139</v>
       </c>
       <c r="H4" t="s">
-        <v>9</v>
+        <v>139</v>
       </c>
       <c r="I4" t="s">
         <v>24</v>
@@ -3782,51 +3780,51 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="5"/>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" t="s">
         <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" t="s">
-        <v>10</v>
       </c>
       <c r="N5" t="s">
         <v>17</v>
       </c>
       <c r="O5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q5" t="s">
         <v>19</v>
@@ -3875,10 +3873,10 @@
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="5"/>
       <c r="C6">
         <v>3</v>
       </c>
@@ -3968,385 +3966,475 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="5"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4"/>
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4"/>
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4"/>
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
+      <c r="A78" s="5"/>
+      <c r="B78" s="5"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" s="4"/>
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
-      <c r="B83" s="4"/>
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
-      <c r="B84" s="4"/>
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4"/>
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
-      <c r="B86" s="4"/>
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4"/>
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4"/>
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4"/>
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
-      <c r="B93" s="4"/>
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4"/>
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
-      <c r="B95" s="4"/>
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
-      <c r="B96" s="4"/>
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
-      <c r="B98" s="4"/>
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="106">
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
@@ -4363,96 +4451,6 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trainer parties up to Roxanne
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CF7CD2-F542-47F4-9A3F-B77A72F0D040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187A938A-F874-4F47-92CB-F7A633B600F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2550" windowWidth="15300" windowHeight="7875" activeTab="1" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
+    <workbookView xWindow="2550" yWindow="2550" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
   <sheets>
     <sheet name="Regional Dex" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="282">
   <si>
     <t>Land</t>
   </si>
@@ -931,10 +931,10 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1291,7 +1291,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
   <dimension ref="A1:F260"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1573,6 +1575,9 @@
       <c r="B24" t="s">
         <v>18</v>
       </c>
+      <c r="C24" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1581,6 +1586,9 @@
       <c r="B25" t="s">
         <v>50</v>
       </c>
+      <c r="C25" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1589,6 +1597,9 @@
       <c r="B26" t="s">
         <v>51</v>
       </c>
+      <c r="C26" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1629,6 +1640,9 @@
       <c r="B31" t="s">
         <v>30</v>
       </c>
+      <c r="C31" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -1636,6 +1650,9 @@
       </c>
       <c r="B32" t="s">
         <v>56</v>
+      </c>
+      <c r="C32" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -3471,19 +3488,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A925BAE-2E1E-4059-B9E1-CE8878C0DE7F}">
   <dimension ref="A1:AK100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="5"/>
       <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3498,40 +3515,40 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4" t="s">
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4" t="s">
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4" t="s">
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3636,10 +3653,10 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -3687,10 +3704,10 @@
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="4"/>
       <c r="C4">
         <v>3</v>
       </c>
@@ -3780,10 +3797,10 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5">
         <v>3</v>
       </c>
@@ -3873,10 +3890,10 @@
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="4"/>
       <c r="C6">
         <v>3</v>
       </c>
@@ -3966,475 +3983,385 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="5"/>
-      <c r="B77" s="5"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="5"/>
-      <c r="B78" s="5"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
-      <c r="B85" s="5"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
-      <c r="B86" s="5"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-      <c r="B87" s="5"/>
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="B89" s="5"/>
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="5"/>
-      <c r="B95" s="5"/>
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="5"/>
-      <c r="B96" s="5"/>
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="5"/>
-      <c r="B97" s="5"/>
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-      <c r="B98" s="5"/>
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="5"/>
-      <c r="B99" s="5"/>
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="5"/>
-      <c r="B100" s="5"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="106">
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
     <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
@@ -4451,6 +4378,96 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update wild encounters and trainer parties up to Route 116
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187A938A-F874-4F47-92CB-F7A633B600F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4933379-2D36-485E-92AB-70002293706F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2550" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
+    <workbookView xWindow="2550" yWindow="2550" windowWidth="15300" windowHeight="7875" activeTab="1" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
   <sheets>
     <sheet name="Regional Dex" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="285">
   <si>
     <t>Land</t>
   </si>
@@ -883,6 +883,15 @@
   </si>
   <si>
     <t>Abilities</t>
+  </si>
+  <si>
+    <t>Route 116</t>
+  </si>
+  <si>
+    <t>Machop</t>
+  </si>
+  <si>
+    <t>Abra</t>
   </si>
 </sst>
 </file>
@@ -1291,9 +1300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
   <dimension ref="A1:F260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3488,8 +3495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A925BAE-2E1E-4059-B9E1-CE8878C0DE7F}">
   <dimension ref="A1:AK100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3895,10 +3902,10 @@
       </c>
       <c r="B6" s="4"/>
       <c r="C6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -3907,7 +3914,7 @@
         <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
         <v>19</v>
@@ -3916,7 +3923,7 @@
         <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="K6" t="s">
         <v>30</v>
@@ -3987,10 +3994,96 @@
         <v>274</v>
       </c>
       <c r="B7" s="4"/>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" t="s">
+        <v>71</v>
+      </c>
+      <c r="N7" t="s">
+        <v>222</v>
+      </c>
+      <c r="O7" t="s">
+        <v>71</v>
+      </c>
+      <c r="P7" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>282</v>
+      </c>
       <c r="B8" s="4"/>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H8" t="s">
+        <v>152</v>
+      </c>
+      <c r="I8" t="s">
+        <v>283</v>
+      </c>
+      <c r="J8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" t="s">
+        <v>284</v>
+      </c>
+      <c r="P8" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>

</xml_diff>

<commit_message>
Add mons back into regional dex
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4933379-2D36-485E-92AB-70002293706F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECDBC17-AF74-49D1-9A02-DE44CD92021D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2550" windowWidth="15300" windowHeight="7875" activeTab="1" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
+    <workbookView xWindow="2550" yWindow="2550" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
   <sheets>
     <sheet name="Regional Dex" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="293">
   <si>
     <t>Land</t>
   </si>
@@ -892,6 +892,30 @@
   </si>
   <si>
     <t>Abra</t>
+  </si>
+  <si>
+    <t>Machoke</t>
+  </si>
+  <si>
+    <t>Machamp</t>
+  </si>
+  <si>
+    <t>Kadabra</t>
+  </si>
+  <si>
+    <t>Alakazam</t>
+  </si>
+  <si>
+    <t>Grimer</t>
+  </si>
+  <si>
+    <t>Muk</t>
+  </si>
+  <si>
+    <t>Koffing</t>
+  </si>
+  <si>
+    <t>Weezing</t>
   </si>
 </sst>
 </file>
@@ -1298,9 +1322,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
-  <dimension ref="A1:F260"/>
+  <dimension ref="A1:F270"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1835,7 +1861,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>74</v>
+        <v>284</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1843,7 +1869,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>75</v>
+        <v>287</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1851,7 +1877,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>76</v>
+        <v>288</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1859,7 +1885,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1867,7 +1893,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1875,7 +1901,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1883,7 +1909,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1891,7 +1917,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1899,7 +1925,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1907,7 +1933,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1915,7 +1941,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1923,7 +1949,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1931,7 +1957,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1939,7 +1965,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1947,7 +1973,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1955,7 +1981,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1963,7 +1989,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1971,7 +1997,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1979,7 +2005,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1987,7 +2013,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1995,7 +2021,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2003,7 +2029,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2011,7 +2037,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2019,7 +2045,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2027,7 +2053,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2035,7 +2061,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2043,7 +2069,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -2051,7 +2077,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2059,7 +2085,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -2067,7 +2093,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -2075,7 +2101,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2083,7 +2109,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -2091,7 +2117,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -2099,7 +2125,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2107,7 +2133,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -2115,7 +2141,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2123,7 +2149,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>106</v>
+        <v>25</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2131,7 +2157,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2139,7 +2165,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2147,7 +2173,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2155,7 +2181,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2163,7 +2189,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -2171,7 +2197,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2179,7 +2205,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -2187,7 +2213,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -2195,7 +2221,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2203,7 +2229,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2211,7 +2237,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -2219,7 +2245,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2227,7 +2253,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2235,7 +2261,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2243,7 +2269,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2251,7 +2277,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>122</v>
+        <v>283</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2259,7 +2285,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>123</v>
+        <v>285</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2267,7 +2293,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>124</v>
+        <v>286</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2275,7 +2301,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -2283,7 +2309,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -2291,7 +2317,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2299,7 +2325,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -2307,7 +2333,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -2315,7 +2341,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2323,7 +2349,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -2331,7 +2357,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -2339,7 +2365,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -2347,7 +2373,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -2355,7 +2381,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -2363,7 +2389,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -2371,7 +2397,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -2379,7 +2405,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -2387,7 +2413,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2395,7 +2421,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -2403,7 +2429,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -2411,7 +2437,7 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2419,7 +2445,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>27</v>
+        <v>137</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -2427,7 +2453,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -2435,7 +2461,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2443,7 +2469,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -2451,7 +2477,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -2459,7 +2485,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>146</v>
+        <v>28</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -2467,7 +2493,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>147</v>
+        <v>27</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -2475,7 +2501,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -2483,7 +2509,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -2491,7 +2517,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -2499,7 +2525,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -2507,7 +2533,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -2515,7 +2541,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -2523,7 +2549,7 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -2531,7 +2557,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>155</v>
+        <v>289</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -2539,7 +2565,7 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>156</v>
+        <v>290</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -2547,7 +2573,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>157</v>
+        <v>291</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -2555,7 +2581,7 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>158</v>
+        <v>292</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -2563,7 +2589,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -2571,7 +2597,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -2579,7 +2605,7 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -2587,7 +2613,7 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -2595,7 +2621,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -2603,7 +2629,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -2611,7 +2637,7 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -2619,7 +2645,7 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -2627,7 +2653,7 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -2635,7 +2661,7 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -2643,7 +2669,7 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -2651,7 +2677,7 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -2659,7 +2685,7 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -2667,7 +2693,7 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -2675,7 +2701,7 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -2683,7 +2709,7 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -2691,7 +2717,7 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -2699,7 +2725,7 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -2707,7 +2733,7 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -2715,7 +2741,7 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -2723,7 +2749,7 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>22</v>
+        <v>169</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -2731,7 +2757,7 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -2739,7 +2765,7 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -2747,7 +2773,7 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -2755,7 +2781,7 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -2763,7 +2789,7 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -2771,7 +2797,7 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -2779,7 +2805,7 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -2787,7 +2813,7 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -2795,7 +2821,7 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -2803,7 +2829,7 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>188</v>
+        <v>22</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -2811,7 +2837,7 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -2819,7 +2845,7 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -2827,7 +2853,7 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -2835,7 +2861,7 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -2843,7 +2869,7 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -2851,7 +2877,7 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -2859,7 +2885,7 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -2867,7 +2893,7 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -2875,7 +2901,7 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -2883,7 +2909,7 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -2891,7 +2917,7 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -2899,7 +2925,7 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -2907,7 +2933,7 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -2915,7 +2941,7 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -2923,7 +2949,7 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -2931,7 +2957,7 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -2939,7 +2965,7 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -2947,7 +2973,7 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -2955,7 +2981,7 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -2963,7 +2989,7 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -2971,7 +2997,7 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -2979,7 +3005,7 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -2987,7 +3013,7 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -2995,7 +3021,7 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -3003,7 +3029,7 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -3011,7 +3037,7 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -3019,7 +3045,7 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -3027,7 +3053,7 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -3035,7 +3061,7 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -3043,7 +3069,7 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
@@ -3051,7 +3077,7 @@
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
@@ -3059,7 +3085,7 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -3067,7 +3093,7 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
@@ -3075,7 +3101,7 @@
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
@@ -3083,7 +3109,7 @@
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
@@ -3091,7 +3117,7 @@
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -3099,7 +3125,7 @@
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
@@ -3107,7 +3133,7 @@
         <v>212</v>
       </c>
       <c r="B213" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
@@ -3115,7 +3141,7 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
@@ -3123,7 +3149,7 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
@@ -3131,7 +3157,7 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
@@ -3139,7 +3165,7 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
@@ -3147,7 +3173,7 @@
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
@@ -3155,7 +3181,7 @@
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -3163,7 +3189,7 @@
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
@@ -3171,7 +3197,7 @@
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
@@ -3179,7 +3205,7 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
@@ -3187,7 +3213,7 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
@@ -3195,7 +3221,7 @@
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
@@ -3203,7 +3229,7 @@
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
@@ -3211,7 +3237,7 @@
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
@@ -3219,7 +3245,7 @@
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
@@ -3227,7 +3253,7 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
@@ -3235,7 +3261,7 @@
         <v>228</v>
       </c>
       <c r="B229" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
@@ -3243,7 +3269,7 @@
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
@@ -3251,7 +3277,7 @@
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -3259,7 +3285,7 @@
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
@@ -3267,7 +3293,7 @@
         <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
@@ -3275,7 +3301,7 @@
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -3283,7 +3309,7 @@
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
@@ -3291,7 +3317,7 @@
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
@@ -3299,7 +3325,7 @@
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -3307,7 +3333,7 @@
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
@@ -3315,7 +3341,7 @@
         <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
@@ -3323,7 +3349,7 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
@@ -3331,7 +3357,7 @@
         <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
@@ -3339,7 +3365,7 @@
         <v>241</v>
       </c>
       <c r="B242" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
@@ -3347,7 +3373,7 @@
         <v>242</v>
       </c>
       <c r="B243" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
@@ -3355,7 +3381,7 @@
         <v>243</v>
       </c>
       <c r="B244" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
@@ -3363,7 +3389,7 @@
         <v>244</v>
       </c>
       <c r="B245" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
@@ -3371,7 +3397,7 @@
         <v>245</v>
       </c>
       <c r="B246" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -3379,7 +3405,7 @@
         <v>246</v>
       </c>
       <c r="B247" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
@@ -3387,7 +3413,7 @@
         <v>247</v>
       </c>
       <c r="B248" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
@@ -3395,7 +3421,7 @@
         <v>248</v>
       </c>
       <c r="B249" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
@@ -3403,7 +3429,7 @@
         <v>249</v>
       </c>
       <c r="B250" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
@@ -3411,7 +3437,7 @@
         <v>250</v>
       </c>
       <c r="B251" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
@@ -3419,7 +3445,7 @@
         <v>251</v>
       </c>
       <c r="B252" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
@@ -3427,7 +3453,7 @@
         <v>252</v>
       </c>
       <c r="B253" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
@@ -3435,7 +3461,7 @@
         <v>253</v>
       </c>
       <c r="B254" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
@@ -3443,7 +3469,7 @@
         <v>254</v>
       </c>
       <c r="B255" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
@@ -3451,7 +3477,7 @@
         <v>255</v>
       </c>
       <c r="B256" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
@@ -3459,7 +3485,7 @@
         <v>256</v>
       </c>
       <c r="B257" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
@@ -3467,7 +3493,7 @@
         <v>257</v>
       </c>
       <c r="B258" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
@@ -3475,7 +3501,7 @@
         <v>258</v>
       </c>
       <c r="B259" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
@@ -3483,6 +3509,74 @@
         <v>259</v>
       </c>
       <c r="B260" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>260</v>
+      </c>
+      <c r="B261" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>261</v>
+      </c>
+      <c r="B262" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>262</v>
+      </c>
+      <c r="B263" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>263</v>
+      </c>
+      <c r="B264" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>264</v>
+      </c>
+      <c r="B265" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>265</v>
+      </c>
+      <c r="B266" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B267" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B268" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B269" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B270" t="s">
         <v>273</v>
       </c>
     </row>
@@ -3495,8 +3589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A925BAE-2E1E-4059-B9E1-CE8878C0DE7F}">
   <dimension ref="A1:AK100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add learnsets for Shroomish and Slakoth families
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28516"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B152C12-2DCF-469C-BDEA-AA9821061375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E8B8EA-4666-4469-9317-B2EA260FB784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2595" yWindow="2595" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="293">
   <si>
     <t>Land</t>
   </si>
@@ -964,10 +964,10 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1324,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
   <dimension ref="A1:F270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A260" workbookViewId="0">
-      <selection activeCell="A270" sqref="A270"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,55 +1688,73 @@
         <v>280</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1744,7 +1762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1752,7 +1770,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1760,23 +1778,29 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1784,7 +1808,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1792,47 +1816,62 @@
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1840,7 +1879,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1848,7 +1887,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1856,7 +1895,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1864,7 +1903,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1872,7 +1911,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1880,7 +1919,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1888,7 +1927,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1896,7 +1935,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1904,7 +1943,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1912,7 +1951,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1920,7 +1959,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1928,7 +1967,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1936,7 +1975,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3602,18 +3641,18 @@
   <dimension ref="A1:AK100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="5"/>
       <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3628,40 +3667,40 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4" t="s">
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4" t="s">
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4" t="s">
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3766,10 +3805,10 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -3817,10 +3856,10 @@
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="4"/>
       <c r="C4">
         <v>3</v>
       </c>
@@ -3910,10 +3949,10 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5">
         <v>3</v>
       </c>
@@ -4003,10 +4042,10 @@
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="4"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -4096,10 +4135,10 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="4"/>
       <c r="C7">
         <v>5</v>
       </c>
@@ -4144,10 +4183,10 @@
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
       <c r="C8">
         <v>8</v>
       </c>
@@ -4192,465 +4231,375 @@
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="5"/>
-      <c r="B77" s="5"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="5"/>
-      <c r="B78" s="5"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
-      <c r="B85" s="5"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
-      <c r="B86" s="5"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-      <c r="B87" s="5"/>
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="B89" s="5"/>
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="5"/>
-      <c r="B95" s="5"/>
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="5"/>
-      <c r="B96" s="5"/>
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="5"/>
-      <c r="B97" s="5"/>
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-      <c r="B98" s="5"/>
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="5"/>
-      <c r="B99" s="5"/>
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="5"/>
-      <c r="B100" s="5"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="106">
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
     <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
@@ -4667,6 +4616,96 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add learnsets for Nincada and Whismur families
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28604"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E8B8EA-4666-4469-9317-B2EA260FB784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F982DD23-EA16-41AD-AD81-4D62D7F50804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2595" yWindow="2595" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="293">
   <si>
     <t>Land</t>
   </si>
@@ -964,10 +964,10 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1324,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
   <dimension ref="A1:F270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1926,6 +1926,9 @@
       <c r="B57" t="s">
         <v>74</v>
       </c>
+      <c r="C57" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -1934,6 +1937,9 @@
       <c r="B58" t="s">
         <v>75</v>
       </c>
+      <c r="C58" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
@@ -1942,6 +1948,9 @@
       <c r="B59" t="s">
         <v>76</v>
       </c>
+      <c r="C59" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
@@ -1950,6 +1959,9 @@
       <c r="B60" t="s">
         <v>77</v>
       </c>
+      <c r="C60" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
@@ -1958,6 +1970,9 @@
       <c r="B61" t="s">
         <v>78</v>
       </c>
+      <c r="C61" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
@@ -1965,6 +1980,9 @@
       </c>
       <c r="B62" t="s">
         <v>79</v>
+      </c>
+      <c r="C62" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -3647,12 +3665,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="4"/>
       <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3667,40 +3685,40 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5" t="s">
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5" t="s">
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5" t="s">
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5" t="s">
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3805,10 +3823,10 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="5"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -3856,10 +3874,10 @@
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="5"/>
       <c r="C4">
         <v>3</v>
       </c>
@@ -3949,10 +3967,10 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="5"/>
       <c r="C5">
         <v>3</v>
       </c>
@@ -4042,10 +4060,10 @@
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="5"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -4135,10 +4153,10 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="5"/>
       <c r="C7">
         <v>5</v>
       </c>
@@ -4183,10 +4201,10 @@
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8">
         <v>8</v>
       </c>
@@ -4231,375 +4249,465 @@
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4"/>
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4"/>
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4"/>
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
+      <c r="A78" s="5"/>
+      <c r="B78" s="5"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" s="4"/>
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
-      <c r="B83" s="4"/>
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
-      <c r="B84" s="4"/>
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4"/>
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
-      <c r="B86" s="4"/>
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4"/>
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4"/>
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4"/>
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
-      <c r="B93" s="4"/>
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4"/>
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
-      <c r="B95" s="4"/>
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
-      <c r="B96" s="4"/>
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
-      <c r="B98" s="4"/>
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="106">
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
@@ -4616,96 +4724,6 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add learnsets up to Makuhita
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F982DD23-EA16-41AD-AD81-4D62D7F50804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787D8442-F466-45D4-B48F-BD3526EEC8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2595" yWindow="2595" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="293">
   <si>
     <t>Land</t>
   </si>
@@ -964,10 +964,10 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1324,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
   <dimension ref="A1:F270"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1641,6 +1641,9 @@
       <c r="B27" t="s">
         <v>52</v>
       </c>
+      <c r="C27" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1649,6 +1652,9 @@
       <c r="B28" t="s">
         <v>53</v>
       </c>
+      <c r="C28" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -1657,6 +1663,9 @@
       <c r="B29" t="s">
         <v>54</v>
       </c>
+      <c r="C29" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -1665,6 +1674,9 @@
       <c r="B30" t="s">
         <v>55</v>
       </c>
+      <c r="C30" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1761,6 +1773,9 @@
       <c r="B39" t="s">
         <v>15</v>
       </c>
+      <c r="C39" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -1769,6 +1784,9 @@
       <c r="B40" t="s">
         <v>60</v>
       </c>
+      <c r="C40" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -1777,6 +1795,9 @@
       <c r="B41" t="s">
         <v>61</v>
       </c>
+      <c r="C41" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -1878,6 +1899,9 @@
       <c r="B51" t="s">
         <v>71</v>
       </c>
+      <c r="C51" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
@@ -1886,6 +1910,9 @@
       <c r="B52" t="s">
         <v>72</v>
       </c>
+      <c r="C52" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
@@ -1894,6 +1921,9 @@
       <c r="B53" t="s">
         <v>73</v>
       </c>
+      <c r="C53" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
@@ -1902,6 +1932,9 @@
       <c r="B54" t="s">
         <v>284</v>
       </c>
+      <c r="C54" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -1910,6 +1943,9 @@
       <c r="B55" t="s">
         <v>287</v>
       </c>
+      <c r="C55" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
@@ -1917,6 +1953,9 @@
       </c>
       <c r="B56" t="s">
         <v>288</v>
+      </c>
+      <c r="C56" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -3665,12 +3704,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="5"/>
       <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3685,40 +3724,40 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4" t="s">
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4" t="s">
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4" t="s">
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3823,10 +3862,10 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -3874,10 +3913,10 @@
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="4"/>
       <c r="C4">
         <v>3</v>
       </c>
@@ -3967,10 +4006,10 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5">
         <v>3</v>
       </c>
@@ -4060,10 +4099,10 @@
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="4"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -4153,10 +4192,10 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="4"/>
       <c r="C7">
         <v>5</v>
       </c>
@@ -4201,10 +4240,10 @@
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
       <c r="C8">
         <v>8</v>
       </c>
@@ -4249,465 +4288,375 @@
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="5"/>
-      <c r="B77" s="5"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="5"/>
-      <c r="B78" s="5"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
-      <c r="B85" s="5"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
-      <c r="B86" s="5"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-      <c r="B87" s="5"/>
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="B89" s="5"/>
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="5"/>
-      <c r="B95" s="5"/>
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="5"/>
-      <c r="B96" s="5"/>
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="5"/>
-      <c r="B97" s="5"/>
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-      <c r="B98" s="5"/>
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="5"/>
-      <c r="B99" s="5"/>
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="5"/>
-      <c r="B100" s="5"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="106">
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
     <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
@@ -4724,6 +4673,96 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update trainer parties up to museum
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28604"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28702"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Decomps\eva-emerald\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\slashumsonic\decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787D8442-F466-45D4-B48F-BD3526EEC8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236BB84D-90A3-4D38-A6EE-DE1229685893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="2595" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
   <sheets>
     <sheet name="Regional Dex" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="300">
   <si>
     <t>Land</t>
   </si>
@@ -916,6 +916,27 @@
   </si>
   <si>
     <t>Weezing</t>
+  </si>
+  <si>
+    <t>Route 106</t>
+  </si>
+  <si>
+    <t>Dewford Town</t>
+  </si>
+  <si>
+    <t>Granite Cave 1F</t>
+  </si>
+  <si>
+    <t>Rusturf Tunnel</t>
+  </si>
+  <si>
+    <t>Granite Cave B1F</t>
+  </si>
+  <si>
+    <t>Granite Cave B2F</t>
+  </si>
+  <si>
+    <t>Granite Cave Steven's Room</t>
   </si>
 </sst>
 </file>
@@ -1324,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
   <dimension ref="A1:F270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
+      <selection activeCell="B239" sqref="B239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3695,10 +3716,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A925BAE-2E1E-4059-B9E1-CE8878C0DE7F}">
-  <dimension ref="A1:AK100"/>
+  <dimension ref="A1:AK101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4269,51 +4290,293 @@
         <v>30</v>
       </c>
       <c r="K8" t="s">
-        <v>30</v>
+        <v>204</v>
       </c>
       <c r="L8" t="s">
-        <v>30</v>
+        <v>204</v>
       </c>
       <c r="M8" t="s">
         <v>10</v>
       </c>
       <c r="N8" t="s">
+        <v>9</v>
+      </c>
+      <c r="O8" t="s">
+        <v>201</v>
+      </c>
+      <c r="P8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" t="s">
+        <v>114</v>
+      </c>
+      <c r="I9" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K9" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" t="s">
+        <v>88</v>
+      </c>
+      <c r="M9" t="s">
+        <v>91</v>
+      </c>
+      <c r="N9" t="s">
+        <v>91</v>
+      </c>
+      <c r="O9" t="s">
+        <v>91</v>
+      </c>
+      <c r="P9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>12</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11">
         <v>10</v>
       </c>
-      <c r="O8" t="s">
+      <c r="D11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" t="s">
+        <v>100</v>
+      </c>
+      <c r="I12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" t="s">
         <v>284</v>
       </c>
-      <c r="P8" t="s">
+      <c r="K12" t="s">
+        <v>80</v>
+      </c>
+      <c r="L12" t="s">
+        <v>80</v>
+      </c>
+      <c r="M12" t="s">
+        <v>88</v>
+      </c>
+      <c r="N12" t="s">
+        <v>88</v>
+      </c>
+      <c r="O12" t="s">
+        <v>88</v>
+      </c>
+      <c r="P12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" t="s">
+        <v>116</v>
+      </c>
+      <c r="H13" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+      <c r="K13" t="s">
+        <v>80</v>
+      </c>
+      <c r="L13" t="s">
+        <v>80</v>
+      </c>
+      <c r="M13" t="s">
+        <v>111</v>
+      </c>
+      <c r="N13" t="s">
+        <v>111</v>
+      </c>
+      <c r="O13" t="s">
+        <v>111</v>
+      </c>
+      <c r="P13" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>298</v>
+      </c>
       <c r="B14" s="4"/>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G14" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" t="s">
+        <v>116</v>
+      </c>
+      <c r="J14" t="s">
+        <v>284</v>
+      </c>
+      <c r="K14" t="s">
+        <v>111</v>
+      </c>
+      <c r="L14" t="s">
+        <v>111</v>
+      </c>
+      <c r="M14" t="s">
+        <v>111</v>
+      </c>
+      <c r="N14" t="s">
+        <v>111</v>
+      </c>
+      <c r="O14" t="s">
+        <v>111</v>
+      </c>
+      <c r="P14" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+      <c r="A15" s="4" t="s">
+        <v>299</v>
+      </c>
       <c r="B15" s="4"/>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" t="s">
+        <v>100</v>
+      </c>
+      <c r="I15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" t="s">
+        <v>284</v>
+      </c>
+      <c r="K15" t="s">
+        <v>80</v>
+      </c>
+      <c r="L15" t="s">
+        <v>80</v>
+      </c>
+      <c r="M15" t="s">
+        <v>116</v>
+      </c>
+      <c r="N15" t="s">
+        <v>116</v>
+      </c>
+      <c r="O15" t="s">
+        <v>116</v>
+      </c>
+      <c r="P15" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
@@ -4655,14 +4918,18 @@
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
     </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="106">
+  <mergeCells count="107">
     <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="E1:P1"/>
     <mergeCell ref="Q1:U1"/>
@@ -4672,97 +4939,98 @@
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A32:B32"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A26:B26"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A44:B44"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A38:B38"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A56:B56"/>
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A50:B50"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="A65:B65"/>
     <mergeCell ref="A66:B66"/>
     <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A68:B68"/>
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A59:B59"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A62:B62"/>
     <mergeCell ref="A75:B75"/>
     <mergeCell ref="A76:B76"/>
     <mergeCell ref="A77:B77"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A80:B80"/>
     <mergeCell ref="A69:B69"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A74:B74"/>
     <mergeCell ref="A87:B87"/>
     <mergeCell ref="A88:B88"/>
     <mergeCell ref="A89:B89"/>
     <mergeCell ref="A90:B90"/>
     <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A92:B92"/>
     <mergeCell ref="A81:B81"/>
     <mergeCell ref="A82:B82"/>
     <mergeCell ref="A83:B83"/>
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A86:B86"/>
     <mergeCell ref="A99:B99"/>
     <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A101:B101"/>
     <mergeCell ref="A93:B93"/>
     <mergeCell ref="A94:B94"/>
     <mergeCell ref="A95:B95"/>
     <mergeCell ref="A96:B96"/>
     <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix remaining TM references
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29107"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\slashumsonic\decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236BB84D-90A3-4D38-A6EE-DE1229685893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF737982-A816-43AF-843D-AA013C90FFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
   <sheets>
     <sheet name="Regional Dex" sheetId="2" r:id="rId1"/>
@@ -985,10 +985,10 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
   <dimension ref="A1:F270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="B239" sqref="B239"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3725,12 +3725,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="4"/>
       <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3745,40 +3745,40 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5" t="s">
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5" t="s">
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5" t="s">
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5" t="s">
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3883,10 +3883,10 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="5"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -3934,10 +3934,10 @@
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="5"/>
       <c r="C4">
         <v>3</v>
       </c>
@@ -4027,10 +4027,10 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="5"/>
       <c r="C5">
         <v>3</v>
       </c>
@@ -4120,10 +4120,10 @@
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="5"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -4213,10 +4213,10 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="5"/>
       <c r="C7">
         <v>5</v>
       </c>
@@ -4261,10 +4261,10 @@
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8">
         <v>8</v>
       </c>
@@ -4309,10 +4309,10 @@
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="5"/>
       <c r="C9">
         <v>8</v>
       </c>
@@ -4357,10 +4357,10 @@
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="5"/>
       <c r="C10">
         <v>8</v>
       </c>
@@ -4375,10 +4375,10 @@
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="5"/>
       <c r="C11">
         <v>10</v>
       </c>
@@ -4387,10 +4387,10 @@
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="5"/>
       <c r="C12">
         <v>6</v>
       </c>
@@ -4435,10 +4435,10 @@
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="5"/>
       <c r="C13">
         <v>9</v>
       </c>
@@ -4483,10 +4483,10 @@
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="5"/>
       <c r="C14">
         <v>10</v>
       </c>
@@ -4531,10 +4531,10 @@
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="5"/>
       <c r="C15">
         <v>6</v>
       </c>
@@ -4579,351 +4579,441 @@
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4"/>
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4"/>
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4"/>
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
+      <c r="A78" s="5"/>
+      <c r="B78" s="5"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" s="4"/>
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
-      <c r="B83" s="4"/>
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
-      <c r="B84" s="4"/>
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4"/>
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
-      <c r="B86" s="4"/>
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4"/>
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4"/>
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4"/>
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
-      <c r="B93" s="4"/>
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4"/>
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
-      <c r="B95" s="4"/>
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
-      <c r="B96" s="4"/>
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
-      <c r="B98" s="4"/>
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="4"/>
-      <c r="B101" s="4"/>
+      <c r="A101" s="5"/>
+      <c r="B101" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="107">
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
@@ -4941,96 +5031,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A98:B98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Learnsets up to Gyarados
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29115"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\slashumsonic\decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF737982-A816-43AF-843D-AA013C90FFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0F8A63-DE33-458B-965B-F61F679F46B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="1425" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
   <sheets>
     <sheet name="Regional Dex" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="300">
   <si>
     <t>Land</t>
   </si>
@@ -985,10 +985,10 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
   <dimension ref="A1:F270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2052,6 +2052,9 @@
       <c r="B63" t="s">
         <v>80</v>
       </c>
+      <c r="C63" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
@@ -2060,40 +2063,55 @@
       <c r="B64" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2101,7 +2119,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2109,7 +2127,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2117,7 +2135,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2125,7 +2143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2133,7 +2151,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2141,7 +2159,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2149,7 +2167,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2157,7 +2175,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2165,7 +2183,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2173,7 +2191,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2181,7 +2199,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3725,12 +3743,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="5"/>
       <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3745,40 +3763,40 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4" t="s">
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4" t="s">
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4" t="s">
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3883,10 +3901,10 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -3934,10 +3952,10 @@
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="4"/>
       <c r="C4">
         <v>3</v>
       </c>
@@ -4027,10 +4045,10 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5">
         <v>3</v>
       </c>
@@ -4120,10 +4138,10 @@
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="4"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -4213,10 +4231,10 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="4"/>
       <c r="C7">
         <v>5</v>
       </c>
@@ -4261,10 +4279,10 @@
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
       <c r="C8">
         <v>8</v>
       </c>
@@ -4309,10 +4327,10 @@
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="4"/>
       <c r="C9">
         <v>8</v>
       </c>
@@ -4357,10 +4375,10 @@
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="4"/>
       <c r="C10">
         <v>8</v>
       </c>
@@ -4375,10 +4393,10 @@
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="4"/>
       <c r="C11">
         <v>10</v>
       </c>
@@ -4387,10 +4405,10 @@
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="4"/>
       <c r="C12">
         <v>6</v>
       </c>
@@ -4435,10 +4453,10 @@
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="4"/>
       <c r="C13">
         <v>9</v>
       </c>
@@ -4483,10 +4501,10 @@
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="4"/>
       <c r="C14">
         <v>10</v>
       </c>
@@ -4531,10 +4549,10 @@
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="4"/>
       <c r="C15">
         <v>6</v>
       </c>
@@ -4579,441 +4597,351 @@
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="5"/>
-      <c r="B77" s="5"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="5"/>
-      <c r="B78" s="5"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
-      <c r="B85" s="5"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
-      <c r="B86" s="5"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-      <c r="B87" s="5"/>
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="B89" s="5"/>
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="5"/>
-      <c r="B95" s="5"/>
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="5"/>
-      <c r="B96" s="5"/>
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="5"/>
-      <c r="B97" s="5"/>
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-      <c r="B98" s="5"/>
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="5"/>
-      <c r="B99" s="5"/>
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="5"/>
-      <c r="B100" s="5"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="5"/>
-      <c r="B101" s="5"/>
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
@@ -5031,6 +4959,96 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Learnsets up to Probopass
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\slashumsonic\decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0F8A63-DE33-458B-965B-F61F679F46B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC3F2DA-92D6-4168-BB56-BB0223405F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1770" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
+    <workbookView xWindow="2115" yWindow="2115" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
   <sheets>
     <sheet name="Regional Dex" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="300">
   <si>
     <t>Land</t>
   </si>
@@ -985,10 +985,10 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
   <dimension ref="A1:F270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2134,6 +2134,9 @@
       <c r="B71" t="s">
         <v>86</v>
       </c>
+      <c r="C71" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
@@ -2142,6 +2145,9 @@
       <c r="B72" t="s">
         <v>19</v>
       </c>
+      <c r="C72" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
@@ -2150,6 +2156,9 @@
       <c r="B73" t="s">
         <v>87</v>
       </c>
+      <c r="C73" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
@@ -2158,6 +2167,9 @@
       <c r="B74" t="s">
         <v>88</v>
       </c>
+      <c r="C74" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
@@ -2166,6 +2178,9 @@
       <c r="B75" t="s">
         <v>89</v>
       </c>
+      <c r="C75" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
@@ -2174,6 +2189,9 @@
       <c r="B76" t="s">
         <v>90</v>
       </c>
+      <c r="C76" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
@@ -2182,6 +2200,9 @@
       <c r="B77" t="s">
         <v>91</v>
       </c>
+      <c r="C77" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
@@ -2190,6 +2211,9 @@
       <c r="B78" t="s">
         <v>92</v>
       </c>
+      <c r="C78" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
@@ -2198,6 +2222,9 @@
       <c r="B79" t="s">
         <v>93</v>
       </c>
+      <c r="C79" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
@@ -2206,32 +2233,44 @@
       <c r="B80" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2239,7 +2278,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2247,7 +2286,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2255,7 +2294,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2263,7 +2302,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2271,7 +2310,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2279,7 +2318,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2287,7 +2326,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2295,7 +2334,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2303,7 +2342,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2311,7 +2350,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2319,7 +2358,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2327,7 +2366,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3743,12 +3782,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="4"/>
       <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3763,40 +3802,40 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5" t="s">
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5" t="s">
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5" t="s">
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5" t="s">
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3901,10 +3940,10 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="5"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -3952,10 +3991,10 @@
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="5"/>
       <c r="C4">
         <v>3</v>
       </c>
@@ -4045,10 +4084,10 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="5"/>
       <c r="C5">
         <v>3</v>
       </c>
@@ -4138,10 +4177,10 @@
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="5"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -4231,10 +4270,10 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="5"/>
       <c r="C7">
         <v>5</v>
       </c>
@@ -4279,10 +4318,10 @@
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8">
         <v>8</v>
       </c>
@@ -4327,10 +4366,10 @@
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="5"/>
       <c r="C9">
         <v>8</v>
       </c>
@@ -4375,10 +4414,10 @@
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="5"/>
       <c r="C10">
         <v>8</v>
       </c>
@@ -4393,10 +4432,10 @@
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="5"/>
       <c r="C11">
         <v>10</v>
       </c>
@@ -4405,10 +4444,10 @@
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="5"/>
       <c r="C12">
         <v>6</v>
       </c>
@@ -4453,10 +4492,10 @@
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="5"/>
       <c r="C13">
         <v>9</v>
       </c>
@@ -4501,10 +4540,10 @@
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="5"/>
       <c r="C14">
         <v>10</v>
       </c>
@@ -4549,10 +4588,10 @@
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="5"/>
       <c r="C15">
         <v>6</v>
       </c>
@@ -4597,351 +4636,441 @@
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4"/>
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4"/>
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4"/>
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
+      <c r="A78" s="5"/>
+      <c r="B78" s="5"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" s="4"/>
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
-      <c r="B83" s="4"/>
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
-      <c r="B84" s="4"/>
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4"/>
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
-      <c r="B86" s="4"/>
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4"/>
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4"/>
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4"/>
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
-      <c r="B93" s="4"/>
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4"/>
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
-      <c r="B95" s="4"/>
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
-      <c r="B96" s="4"/>
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
-      <c r="B98" s="4"/>
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="4"/>
-      <c r="B101" s="4"/>
+      <c r="A101" s="5"/>
+      <c r="B101" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="107">
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
@@ -4959,96 +5088,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A98:B98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Learnsets up to Sableye
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\slashumsonic\decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC3F2DA-92D6-4168-BB56-BB0223405F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E59114-F74F-4EEF-8369-2E88F518440C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="2115" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
+    <workbookView xWindow="2460" yWindow="2460" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
   <sheets>
     <sheet name="Regional Dex" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="300">
   <si>
     <t>Land</t>
   </si>
@@ -985,10 +985,10 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
   <dimension ref="A1:F270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,6 +2277,9 @@
       <c r="B84" t="s">
         <v>98</v>
       </c>
+      <c r="C84" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
@@ -2285,6 +2288,9 @@
       <c r="B85" t="s">
         <v>99</v>
       </c>
+      <c r="C85" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
@@ -2293,6 +2299,9 @@
       <c r="B86" t="s">
         <v>100</v>
       </c>
+      <c r="C86" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
@@ -2301,6 +2310,9 @@
       <c r="B87" t="s">
         <v>101</v>
       </c>
+      <c r="C87" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
@@ -2309,6 +2321,9 @@
       <c r="B88" t="s">
         <v>102</v>
       </c>
+      <c r="C88" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
@@ -2317,6 +2332,9 @@
       <c r="B89" t="s">
         <v>103</v>
       </c>
+      <c r="C89" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
@@ -2325,6 +2343,9 @@
       <c r="B90" t="s">
         <v>25</v>
       </c>
+      <c r="C90" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
@@ -2333,6 +2354,9 @@
       <c r="B91" t="s">
         <v>104</v>
       </c>
+      <c r="C91" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
@@ -2341,6 +2365,9 @@
       <c r="B92" t="s">
         <v>105</v>
       </c>
+      <c r="C92" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
@@ -2349,6 +2376,9 @@
       <c r="B93" t="s">
         <v>106</v>
       </c>
+      <c r="C93" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
@@ -2357,6 +2387,9 @@
       <c r="B94" t="s">
         <v>107</v>
       </c>
+      <c r="C94" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
@@ -2365,6 +2398,9 @@
       <c r="B95" t="s">
         <v>108</v>
       </c>
+      <c r="C95" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
@@ -2373,24 +2409,33 @@
       <c r="B96" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2398,7 +2443,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2406,7 +2451,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2414,7 +2459,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2422,7 +2467,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2430,7 +2475,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2438,7 +2483,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2446,7 +2491,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2454,7 +2499,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2462,7 +2507,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2470,7 +2515,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2478,7 +2523,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2486,7 +2531,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2494,7 +2539,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3782,12 +3827,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="5"/>
       <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3802,40 +3847,40 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4" t="s">
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4" t="s">
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4" t="s">
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3940,10 +3985,10 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -3991,10 +4036,10 @@
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="4"/>
       <c r="C4">
         <v>3</v>
       </c>
@@ -4084,10 +4129,10 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5">
         <v>3</v>
       </c>
@@ -4177,10 +4222,10 @@
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="4"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -4270,10 +4315,10 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="4"/>
       <c r="C7">
         <v>5</v>
       </c>
@@ -4318,10 +4363,10 @@
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
       <c r="C8">
         <v>8</v>
       </c>
@@ -4366,10 +4411,10 @@
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="4"/>
       <c r="C9">
         <v>8</v>
       </c>
@@ -4414,10 +4459,10 @@
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="4"/>
       <c r="C10">
         <v>8</v>
       </c>
@@ -4432,10 +4477,10 @@
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="4"/>
       <c r="C11">
         <v>10</v>
       </c>
@@ -4444,10 +4489,10 @@
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="4"/>
       <c r="C12">
         <v>6</v>
       </c>
@@ -4492,10 +4537,10 @@
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="4"/>
       <c r="C13">
         <v>9</v>
       </c>
@@ -4540,10 +4585,10 @@
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="4"/>
       <c r="C14">
         <v>10</v>
       </c>
@@ -4588,10 +4633,10 @@
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="4"/>
       <c r="C15">
         <v>6</v>
       </c>
@@ -4636,441 +4681,351 @@
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="5"/>
-      <c r="B77" s="5"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="5"/>
-      <c r="B78" s="5"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
-      <c r="B85" s="5"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
-      <c r="B86" s="5"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-      <c r="B87" s="5"/>
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="B89" s="5"/>
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="5"/>
-      <c r="B95" s="5"/>
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="5"/>
-      <c r="B96" s="5"/>
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="5"/>
-      <c r="B97" s="5"/>
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-      <c r="B98" s="5"/>
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="5"/>
-      <c r="B99" s="5"/>
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="5"/>
-      <c r="B100" s="5"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="5"/>
-      <c r="B101" s="5"/>
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
@@ -5088,6 +5043,96 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Learnsets up to Illumise
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\slashumsonic\decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E59114-F74F-4EEF-8369-2E88F518440C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3633F56F-5C9E-4D0A-AC6E-6A6527C4D224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="2460" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
+    <workbookView xWindow="2805" yWindow="2805" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
   <sheets>
     <sheet name="Regional Dex" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="300">
   <si>
     <t>Land</t>
   </si>
@@ -985,10 +985,10 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
   <dimension ref="A1:F270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2442,6 +2442,9 @@
       <c r="B99" t="s">
         <v>112</v>
       </c>
+      <c r="C99" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
@@ -2450,6 +2453,9 @@
       <c r="B100" t="s">
         <v>113</v>
       </c>
+      <c r="C100" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
@@ -2458,6 +2464,9 @@
       <c r="B101" t="s">
         <v>114</v>
       </c>
+      <c r="C101" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
@@ -2466,6 +2475,9 @@
       <c r="B102" t="s">
         <v>115</v>
       </c>
+      <c r="C102" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
@@ -2474,6 +2486,9 @@
       <c r="B103" t="s">
         <v>116</v>
       </c>
+      <c r="C103" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
@@ -2482,6 +2497,9 @@
       <c r="B104" t="s">
         <v>117</v>
       </c>
+      <c r="C104" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
@@ -2490,6 +2508,9 @@
       <c r="B105" t="s">
         <v>118</v>
       </c>
+      <c r="C105" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
@@ -2498,6 +2519,9 @@
       <c r="B106" t="s">
         <v>283</v>
       </c>
+      <c r="C106" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
@@ -2506,6 +2530,9 @@
       <c r="B107" t="s">
         <v>285</v>
       </c>
+      <c r="C107" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
@@ -2514,6 +2541,9 @@
       <c r="B108" t="s">
         <v>286</v>
       </c>
+      <c r="C108" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
@@ -2522,6 +2552,9 @@
       <c r="B109" t="s">
         <v>119</v>
       </c>
+      <c r="C109" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
@@ -2530,6 +2563,9 @@
       <c r="B110" t="s">
         <v>120</v>
       </c>
+      <c r="C110" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
@@ -2538,6 +2574,9 @@
       <c r="B111" t="s">
         <v>121</v>
       </c>
+      <c r="C111" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
@@ -2546,64 +2585,88 @@
       <c r="B112" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
       <c r="B113" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
       <c r="B114" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
       <c r="B115" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
       <c r="B116" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
       <c r="B117" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
       <c r="B118" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
       <c r="B119" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2611,7 +2674,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2619,7 +2682,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -2627,7 +2690,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -2635,7 +2698,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -2643,7 +2706,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -2651,7 +2714,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -2659,7 +2722,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -2667,7 +2730,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -3827,12 +3890,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="4"/>
       <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3847,40 +3910,40 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5" t="s">
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5" t="s">
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5" t="s">
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5" t="s">
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3985,10 +4048,10 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="5"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -4036,10 +4099,10 @@
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="5"/>
       <c r="C4">
         <v>3</v>
       </c>
@@ -4129,10 +4192,10 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="5"/>
       <c r="C5">
         <v>3</v>
       </c>
@@ -4222,10 +4285,10 @@
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="5"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -4315,10 +4378,10 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="5"/>
       <c r="C7">
         <v>5</v>
       </c>
@@ -4363,10 +4426,10 @@
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8">
         <v>8</v>
       </c>
@@ -4411,10 +4474,10 @@
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="5"/>
       <c r="C9">
         <v>8</v>
       </c>
@@ -4459,10 +4522,10 @@
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="5"/>
       <c r="C10">
         <v>8</v>
       </c>
@@ -4477,10 +4540,10 @@
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="5"/>
       <c r="C11">
         <v>10</v>
       </c>
@@ -4489,10 +4552,10 @@
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="5"/>
       <c r="C12">
         <v>6</v>
       </c>
@@ -4537,10 +4600,10 @@
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="5"/>
       <c r="C13">
         <v>9</v>
       </c>
@@ -4585,10 +4648,10 @@
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="5"/>
       <c r="C14">
         <v>10</v>
       </c>
@@ -4633,10 +4696,10 @@
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="5"/>
       <c r="C15">
         <v>6</v>
       </c>
@@ -4681,351 +4744,441 @@
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4"/>
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4"/>
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4"/>
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
+      <c r="A78" s="5"/>
+      <c r="B78" s="5"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" s="4"/>
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
-      <c r="B83" s="4"/>
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
-      <c r="B84" s="4"/>
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4"/>
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
-      <c r="B86" s="4"/>
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4"/>
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4"/>
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4"/>
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
-      <c r="B93" s="4"/>
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4"/>
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
-      <c r="B95" s="4"/>
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
-      <c r="B96" s="4"/>
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
-      <c r="B98" s="4"/>
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="4"/>
-      <c r="B101" s="4"/>
+      <c r="A101" s="5"/>
+      <c r="B101" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="107">
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
@@ -5043,96 +5196,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A98:B98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Learnsets up to Swalot
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\slashumsonic\decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3633F56F-5C9E-4D0A-AC6E-6A6527C4D224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5619EAE-5E9D-4A04-AD2A-0D87FA612B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="2805" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
   <sheets>
     <sheet name="Regional Dex" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="300">
   <si>
     <t>Land</t>
   </si>
@@ -985,10 +985,10 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
   <dimension ref="A1:F270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2721,6 +2721,9 @@
       <c r="B126" t="s">
         <v>136</v>
       </c>
+      <c r="C126" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
@@ -2729,6 +2732,9 @@
       <c r="B127" t="s">
         <v>137</v>
       </c>
+      <c r="C127" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
@@ -2737,24 +2743,33 @@
       <c r="B128" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C128" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
       <c r="B129" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C129" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
       <c r="B130" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C130" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -2762,7 +2777,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -2770,7 +2785,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -2778,7 +2793,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -2786,7 +2801,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -2794,7 +2809,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -2802,7 +2817,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -2810,7 +2825,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -2818,7 +2833,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -2826,7 +2841,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -2834,7 +2849,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -2842,7 +2857,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -2850,7 +2865,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -2858,7 +2873,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -3890,12 +3905,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="5"/>
       <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3910,40 +3925,40 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4" t="s">
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4" t="s">
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4" t="s">
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -4048,10 +4063,10 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -4099,10 +4114,10 @@
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="4"/>
       <c r="C4">
         <v>3</v>
       </c>
@@ -4192,10 +4207,10 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5">
         <v>3</v>
       </c>
@@ -4285,10 +4300,10 @@
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="4"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -4378,10 +4393,10 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="4"/>
       <c r="C7">
         <v>5</v>
       </c>
@@ -4426,10 +4441,10 @@
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
       <c r="C8">
         <v>8</v>
       </c>
@@ -4474,10 +4489,10 @@
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="4"/>
       <c r="C9">
         <v>8</v>
       </c>
@@ -4522,10 +4537,10 @@
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="4"/>
       <c r="C10">
         <v>8</v>
       </c>
@@ -4540,10 +4555,10 @@
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="4"/>
       <c r="C11">
         <v>10</v>
       </c>
@@ -4552,10 +4567,10 @@
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="4"/>
       <c r="C12">
         <v>6</v>
       </c>
@@ -4600,10 +4615,10 @@
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="4"/>
       <c r="C13">
         <v>9</v>
       </c>
@@ -4648,10 +4663,10 @@
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="4"/>
       <c r="C14">
         <v>10</v>
       </c>
@@ -4696,10 +4711,10 @@
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="4"/>
       <c r="C15">
         <v>6</v>
       </c>
@@ -4744,441 +4759,351 @@
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="5"/>
-      <c r="B77" s="5"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="5"/>
-      <c r="B78" s="5"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
-      <c r="B85" s="5"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
-      <c r="B86" s="5"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-      <c r="B87" s="5"/>
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="B89" s="5"/>
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="5"/>
-      <c r="B95" s="5"/>
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="5"/>
-      <c r="B96" s="5"/>
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="5"/>
-      <c r="B97" s="5"/>
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-      <c r="B98" s="5"/>
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="5"/>
-      <c r="B99" s="5"/>
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="5"/>
-      <c r="B100" s="5"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="5"/>
-      <c r="B101" s="5"/>
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
@@ -5196,6 +5121,96 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Misc learnsets up to Eelectross
</commit_message>
<xml_diff>
--- a/docs/Evanescent Emerald Docs.xlsx
+++ b/docs/Evanescent Emerald Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\slashumsonic\decomps\eva-emerald\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E0BD02-1E22-4819-B901-E4E7989F1B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3C122F-0C02-4572-B358-CD8E4204AEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="15300" windowHeight="7875" xr2:uid="{692A5FC6-CC54-47E6-9BC7-B31D3D5D7430}"/>
   </bookViews>
   <sheets>
     <sheet name="Regional Dex" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="300">
   <si>
     <t>Land</t>
   </si>
@@ -985,10 +985,10 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7ABAC1-50AF-4512-AA8E-A0E42184D5E7}">
   <dimension ref="A1:F270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="B245" sqref="B245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2776,6 +2776,9 @@
       <c r="B131" t="s">
         <v>141</v>
       </c>
+      <c r="C131" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
@@ -2784,6 +2787,9 @@
       <c r="B132" t="s">
         <v>28</v>
       </c>
+      <c r="C132" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
@@ -2792,6 +2798,9 @@
       <c r="B133" t="s">
         <v>27</v>
       </c>
+      <c r="C133" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
@@ -2800,6 +2809,9 @@
       <c r="B134" t="s">
         <v>142</v>
       </c>
+      <c r="C134" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
@@ -2808,6 +2820,9 @@
       <c r="B135" t="s">
         <v>143</v>
       </c>
+      <c r="C135" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
@@ -2816,6 +2831,9 @@
       <c r="B136" t="s">
         <v>144</v>
       </c>
+      <c r="C136" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
@@ -2881,7 +2899,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -2889,7 +2907,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -2897,7 +2915,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -2905,7 +2923,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -2913,7 +2931,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -2921,7 +2939,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -2929,7 +2947,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -2937,7 +2955,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -2945,7 +2963,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -2953,7 +2971,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -2961,7 +2979,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -2969,23 +2987,29 @@
         <v>159</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
       <c r="B156" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C156" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
       <c r="B157" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C157" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -2993,7 +3017,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -3001,7 +3025,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -3265,7 +3289,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
@@ -3273,7 +3297,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
@@ -3281,7 +3305,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
@@ -3289,7 +3313,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
@@ -3297,7 +3321,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
@@ -3305,7 +3329,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
@@ -3313,7 +3337,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
@@ -3321,7 +3345,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
@@ -3329,7 +3353,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
@@ -3337,7 +3361,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
@@ -3345,31 +3369,40 @@
         <v>205</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
       <c r="B203" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C203" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
       <c r="B204" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C204" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
       <c r="B205" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C205" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
@@ -3377,7 +3410,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
@@ -3385,7 +3418,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>207</v>
       </c>
@@ -3521,7 +3554,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>224</v>
       </c>
@@ -3529,7 +3562,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>225</v>
       </c>
@@ -3537,7 +3570,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>226</v>
       </c>
@@ -3545,7 +3578,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>227</v>
       </c>
@@ -3553,7 +3586,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>228</v>
       </c>
@@ -3561,7 +3594,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>229</v>
       </c>
@@ -3569,7 +3602,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>230</v>
       </c>
@@ -3577,7 +3610,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>231</v>
       </c>
@@ -3585,7 +3618,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>232</v>
       </c>
@@ -3593,7 +3626,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>233</v>
       </c>
@@ -3601,7 +3634,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>234</v>
       </c>
@@ -3609,7 +3642,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>235</v>
       </c>
@@ -3617,7 +3650,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>236</v>
       </c>
@@ -3625,7 +3658,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>237</v>
       </c>
@@ -3633,7 +3666,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>238</v>
       </c>
@@ -3641,47 +3674,62 @@
         <v>242</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>239</v>
       </c>
       <c r="B240" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C240" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>240</v>
       </c>
       <c r="B241" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C241" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>241</v>
       </c>
       <c r="B242" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C242" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>242</v>
       </c>
       <c r="B243" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C243" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>243</v>
       </c>
       <c r="B244" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C244" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>244</v>
       </c>
@@ -3689,7 +3737,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>245</v>
       </c>
@@ -3697,7 +3745,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>246</v>
       </c>
@@ -3705,7 +3753,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>247</v>
       </c>
@@ -3713,7 +3761,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>248</v>
       </c>
@@ -3721,7 +3769,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>249</v>
       </c>
@@ -3729,7 +3777,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>250</v>
       </c>
@@ -3737,7 +3785,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>251</v>
       </c>
@@ -3745,7 +3793,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>252</v>
       </c>
@@ -3753,7 +3801,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>253</v>
       </c>
@@ -3761,7 +3809,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>254</v>
       </c>
@@ -3769,7 +3817,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>255</v>
       </c>
@@ -3905,12 +3953,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="5"/>
       <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3925,40 +3973,40 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4" t="s">
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4" t="s">
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4" t="s">
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -4063,10 +4111,10 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -4114,10 +4162,10 @@
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="4"/>
       <c r="C4">
         <v>3</v>
       </c>
@@ -4207,10 +4255,10 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5">
         <v>3</v>
       </c>
@@ -4300,10 +4348,10 @@
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="4"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -4393,10 +4441,10 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="4"/>
       <c r="C7">
         <v>5</v>
       </c>
@@ -4441,10 +4489,10 @@
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
       <c r="C8">
         <v>8</v>
       </c>
@@ -4489,10 +4537,10 @@
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="4"/>
       <c r="C9">
         <v>8</v>
       </c>
@@ -4537,10 +4585,10 @@
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="4"/>
       <c r="C10">
         <v>8</v>
       </c>
@@ -4555,10 +4603,10 @@
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="4"/>
       <c r="C11">
         <v>10</v>
       </c>
@@ -4567,10 +4615,10 @@
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="4"/>
       <c r="C12">
         <v>6</v>
       </c>
@@ -4615,10 +4663,10 @@
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="4"/>
       <c r="C13">
         <v>9</v>
       </c>
@@ -4663,10 +4711,10 @@
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="4"/>
       <c r="C14">
         <v>10</v>
       </c>
@@ -4711,10 +4759,10 @@
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="4"/>
       <c r="C15">
         <v>6</v>
       </c>
@@ -4759,441 +4807,351 @@
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="5"/>
-      <c r="B77" s="5"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="5"/>
-      <c r="B78" s="5"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
-      <c r="B85" s="5"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
-      <c r="B86" s="5"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-      <c r="B87" s="5"/>
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="B89" s="5"/>
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="5"/>
-      <c r="B95" s="5"/>
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="5"/>
-      <c r="B96" s="5"/>
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="5"/>
-      <c r="B97" s="5"/>
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-      <c r="B98" s="5"/>
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="5"/>
-      <c r="B99" s="5"/>
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="5"/>
-      <c r="B100" s="5"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="5"/>
-      <c r="B101" s="5"/>
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
@@ -5211,6 +5169,96 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>